<commit_message>
Changed all mohr-coulomb tests (except small_deform1) to use the multisurface stuff.
Also some minor, but important, fiddling with FiniteStrainMultiPlasticity

Fixes #3832
</commit_message>
<xml_diff>
--- a/modules/tensor_mechanics/tests/mohr_coulomb/hard1_2.xlsx
+++ b/modules/tensor_mechanics/tests/mohr_coulomb/hard1_2.xlsx
@@ -15,8 +15,8 @@
     <sheet name="expected2" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="small_deform_hard1" localSheetId="1">small_deform_hard1!$C$4:$M$15</definedName>
-    <definedName name="small_deform_hard1" localSheetId="4">small_deform_hard2!$C$4:$M$15</definedName>
+    <definedName name="small_deform_hard1" localSheetId="1">small_deform_hard1!$C$4:$K$15</definedName>
+    <definedName name="small_deform_hard1" localSheetId="4">small_deform_hard2!$C$4:$K$15</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
   <si>
     <t>time</t>
   </si>
@@ -71,12 +71,6 @@
   </si>
   <si>
     <t>internal</t>
-  </si>
-  <si>
-    <t>max_ps</t>
-  </si>
-  <si>
-    <t>min_ps</t>
   </si>
   <si>
     <t>s_xx</t>
@@ -525,10 +519,10 @@
                 <c:pt idx="1">
                   <c:v>7.0891727672418004E-5</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="General">
+                <c:pt idx="2">
                   <c:v>1.0648444333934E-4</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="General">
+                <c:pt idx="3">
                   <c:v>1.4171936408256E-4</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
@@ -592,14 +586,14 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="52679808"/>
-        <c:axId val="52681344"/>
+        <c:axId val="106490112"/>
+        <c:axId val="106496768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="52679808"/>
+        <c:axId val="106490112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="4.0000000000000007E-4"/>
+          <c:max val="4.0000000000000018E-4"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:title>
@@ -622,12 +616,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52681344"/>
+        <c:crossAx val="106496768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="52681344"/>
+        <c:axId val="106496768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -655,7 +649,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52679808"/>
+        <c:crossAx val="106490112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1089,14 +1083,14 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="112537984"/>
-        <c:axId val="112540288"/>
+        <c:axId val="107203200"/>
+        <c:axId val="107213952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="112537984"/>
+        <c:axId val="107203200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="4.0000000000000018E-4"/>
+          <c:max val="4.0000000000000029E-4"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:title>
@@ -1119,12 +1113,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112540288"/>
+        <c:crossAx val="107213952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="112540288"/>
+        <c:axId val="107213952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -1152,7 +1146,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112537984"/>
+        <c:crossAx val="107203200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1538,21 +1532,23 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O5" sqref="O5:P15"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="3" max="3" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.88671875" customWidth="1"/>
+    <col min="9" max="9" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B1">
         <f>60*PI()/180</f>
@@ -1561,7 +1557,7 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -1595,17 +1591,11 @@
       <c r="K4" t="s">
         <v>8</v>
       </c>
-      <c r="L4" t="s">
+      <c r="O4" t="s">
+        <v>10</v>
+      </c>
+      <c r="P4" t="s">
         <v>9</v>
-      </c>
-      <c r="M4" t="s">
-        <v>10</v>
-      </c>
-      <c r="O4" t="s">
-        <v>12</v>
-      </c>
-      <c r="P4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1636,14 +1626,8 @@
       <c r="K5">
         <v>0</v>
       </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
       <c r="O5">
-        <f>(H5+K5+M5)/3</f>
+        <f>(F5+I5+K5)/3</f>
         <v>0</v>
       </c>
       <c r="P5">
@@ -1664,29 +1648,23 @@
       <c r="F6">
         <v>-0.20177484708821</v>
       </c>
-      <c r="G6">
-        <v>-0.20177484708821999</v>
-      </c>
-      <c r="H6">
+      <c r="G6" s="1">
+        <v>-2.6610018873356999E-16</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1.4320694293883999E-16</v>
+      </c>
+      <c r="I6" s="1">
         <v>-0.20177484708821</v>
       </c>
-      <c r="I6" s="1">
-        <v>-2.6610018873356999E-16</v>
-      </c>
       <c r="J6" s="1">
-        <v>1.4320694293883999E-16</v>
+        <v>1.9931569196681002E-15</v>
       </c>
       <c r="K6">
         <v>-0.20177484708821</v>
       </c>
-      <c r="L6" s="1">
-        <v>1.9931569196681002E-15</v>
-      </c>
-      <c r="M6">
-        <v>-0.20177484708821</v>
-      </c>
       <c r="O6">
-        <f t="shared" ref="O6:O15" si="0">(H6+K6+M6)/3</f>
+        <f t="shared" ref="O6:O15" si="0">(F6+I6+K6)/3</f>
         <v>-0.20177484708821</v>
       </c>
       <c r="P6">
@@ -1707,25 +1685,19 @@
       <c r="F7">
         <v>-1.1908478706457</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
+        <v>4.4646129685896998E-15</v>
+      </c>
+      <c r="H7" s="1">
+        <v>-2.7433752035202E-15</v>
+      </c>
+      <c r="I7" s="1">
         <v>-1.1908478706457</v>
       </c>
-      <c r="H7">
-        <v>-1.1908478706457</v>
-      </c>
-      <c r="I7" s="1">
-        <v>4.4646129685896998E-15</v>
-      </c>
       <c r="J7" s="1">
-        <v>-2.7433752035202E-15</v>
+        <v>-1.4001957486901999E-14</v>
       </c>
       <c r="K7">
-        <v>-1.1908478706457</v>
-      </c>
-      <c r="L7" s="1">
-        <v>-1.4001957486901999E-14</v>
-      </c>
-      <c r="M7">
         <v>-1.1908478706457</v>
       </c>
       <c r="O7">
@@ -1744,31 +1716,25 @@
       <c r="D8" s="1">
         <v>-3.6372852942335E-6</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>1.0648444333934E-4</v>
       </c>
-      <c r="F8">
-        <v>-1.8716283400886999</v>
-      </c>
-      <c r="G8">
+      <c r="F8" s="1">
         <v>-1.8716283400888001</v>
       </c>
-      <c r="H8">
+      <c r="G8" s="1">
+        <v>-1.2523375689706001E-14</v>
+      </c>
+      <c r="H8" s="1">
+        <v>6.7851872147235001E-15</v>
+      </c>
+      <c r="I8" s="1">
         <v>-1.8716283400888001</v>
       </c>
-      <c r="I8" s="1">
-        <v>-1.2523375689706001E-14</v>
-      </c>
       <c r="J8" s="1">
-        <v>6.7851872147235001E-15</v>
-      </c>
-      <c r="K8">
-        <v>-1.8716283400888001</v>
-      </c>
-      <c r="L8" s="1">
         <v>8.9939796018289992E-16</v>
       </c>
-      <c r="M8">
+      <c r="K8" s="1">
         <v>-1.8716283400888001</v>
       </c>
       <c r="O8">
@@ -1787,31 +1753,25 @@
       <c r="D9" s="1">
         <v>-1.1795756502397E-6</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>1.4171936408256E-4</v>
       </c>
       <c r="F9">
         <v>-2.3445362536066998</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1">
+        <v>-2.9312969747734002E-16</v>
+      </c>
+      <c r="H9" s="1">
+        <v>3.2795835294618999E-15</v>
+      </c>
+      <c r="I9" s="1">
         <v>-2.3445362536066998</v>
       </c>
-      <c r="H9">
-        <v>-2.3445362536066998</v>
-      </c>
-      <c r="I9" s="1">
-        <v>-2.9312969747734002E-16</v>
-      </c>
       <c r="J9" s="1">
-        <v>3.2795835294618999E-15</v>
+        <v>-1.1428920798455E-15</v>
       </c>
       <c r="K9">
-        <v>-2.3445362536066998</v>
-      </c>
-      <c r="L9" s="1">
-        <v>-1.1428920798455E-15</v>
-      </c>
-      <c r="M9">
         <v>-2.3445362536066998</v>
       </c>
       <c r="O9">
@@ -1836,25 +1796,19 @@
       <c r="F10">
         <v>-2.6750767616626998</v>
       </c>
-      <c r="G10">
-        <v>-2.6750767616628002</v>
-      </c>
-      <c r="H10">
+      <c r="G10" s="1">
+        <v>2.8985608743443999E-15</v>
+      </c>
+      <c r="H10" s="1">
+        <v>-1.177134492172E-15</v>
+      </c>
+      <c r="I10" s="1">
         <v>-2.6750767616626998</v>
       </c>
-      <c r="I10" s="1">
-        <v>2.8985608743443999E-15</v>
-      </c>
       <c r="J10" s="1">
-        <v>-1.177134492172E-15</v>
+        <v>-2.7759651536128998E-17</v>
       </c>
       <c r="K10">
-        <v>-2.6750767616626998</v>
-      </c>
-      <c r="L10" s="1">
-        <v>-2.7759651536128998E-17</v>
-      </c>
-      <c r="M10">
         <v>-2.6750767616626998</v>
       </c>
       <c r="O10">
@@ -1879,25 +1833,19 @@
       <c r="F11">
         <v>-2.9070846899656</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
+        <v>-7.1084707902443003E-17</v>
+      </c>
+      <c r="H11" s="1">
+        <v>-6.5810398621681002E-16</v>
+      </c>
+      <c r="I11" s="1">
         <v>-2.9070846899656</v>
       </c>
-      <c r="H11">
-        <v>-2.9070846899656</v>
-      </c>
-      <c r="I11" s="1">
-        <v>-7.1084707902443003E-17</v>
-      </c>
       <c r="J11" s="1">
-        <v>-6.5810398621681002E-16</v>
+        <v>-4.5712621012241E-16</v>
       </c>
       <c r="K11">
-        <v>-2.9070846899656</v>
-      </c>
-      <c r="L11" s="1">
-        <v>-4.5712621012241E-16</v>
-      </c>
-      <c r="M11">
         <v>-2.9070846899656</v>
       </c>
       <c r="O11">
@@ -1922,25 +1870,19 @@
       <c r="F12">
         <v>-3.0704069137293</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="1">
+        <v>-1.7431109270737E-15</v>
+      </c>
+      <c r="H12" s="1">
+        <v>4.1951144806457998E-16</v>
+      </c>
+      <c r="I12" s="1">
         <v>-3.0704069137293</v>
       </c>
-      <c r="H12">
-        <v>-3.0704069137293</v>
-      </c>
-      <c r="I12" s="1">
-        <v>-1.7431109270737E-15</v>
-      </c>
       <c r="J12" s="1">
-        <v>4.1951144806457998E-16</v>
+        <v>7.0970258839266001E-16</v>
       </c>
       <c r="K12">
-        <v>-3.0704069137293</v>
-      </c>
-      <c r="L12" s="1">
-        <v>7.0970258839266001E-16</v>
-      </c>
-      <c r="M12">
         <v>-3.0704069137293</v>
       </c>
       <c r="O12">
@@ -1965,25 +1907,19 @@
       <c r="F13">
         <v>-3.1856110269786</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="1">
+        <v>-4.6341963537351002E-17</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1.9731667022862E-16</v>
+      </c>
+      <c r="I13" s="1">
         <v>-3.1856110269786</v>
       </c>
-      <c r="H13">
-        <v>-3.1856110269786</v>
-      </c>
-      <c r="I13" s="1">
-        <v>-4.6341963537351002E-17</v>
-      </c>
       <c r="J13" s="1">
-        <v>1.9731667022862E-16</v>
+        <v>3.1655178427233001E-16</v>
       </c>
       <c r="K13">
-        <v>-3.1856110269786</v>
-      </c>
-      <c r="L13" s="1">
-        <v>3.1655178427233001E-16</v>
-      </c>
-      <c r="M13">
         <v>-3.1856110269786</v>
       </c>
       <c r="O13">
@@ -2008,25 +1944,19 @@
       <c r="F14">
         <v>-3.2669889903131999</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="1">
+        <v>1.4215284479384001E-16</v>
+      </c>
+      <c r="H14" s="1">
+        <v>3.3436436089998999E-16</v>
+      </c>
+      <c r="I14" s="1">
         <v>-3.2669889903131999</v>
       </c>
-      <c r="H14">
-        <v>-3.2669889903131999</v>
-      </c>
-      <c r="I14" s="1">
-        <v>1.4215284479384001E-16</v>
-      </c>
       <c r="J14" s="1">
-        <v>3.3436436089998999E-16</v>
+        <v>7.4580393885422E-17</v>
       </c>
       <c r="K14">
-        <v>-3.2669889903131999</v>
-      </c>
-      <c r="L14" s="1">
-        <v>7.4580393885422E-17</v>
-      </c>
-      <c r="M14">
         <v>-3.2669889903131999</v>
       </c>
       <c r="O14">
@@ -2051,25 +1981,19 @@
       <c r="F15">
         <v>-3.3245301397697</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="1">
+        <v>-3.0573302995836001E-16</v>
+      </c>
+      <c r="H15" s="1">
+        <v>-4.3854632762887998E-18</v>
+      </c>
+      <c r="I15" s="1">
         <v>-3.3245301397697</v>
       </c>
-      <c r="H15">
-        <v>-3.3245301397697</v>
-      </c>
-      <c r="I15" s="1">
-        <v>-3.0573302995836001E-16</v>
-      </c>
       <c r="J15" s="1">
-        <v>-4.3854632762887998E-18</v>
+        <v>1.6995957652293E-16</v>
       </c>
       <c r="K15">
-        <v>-3.3245301397697</v>
-      </c>
-      <c r="L15" s="1">
-        <v>1.6995957652293E-16</v>
-      </c>
-      <c r="M15">
         <v>-3.3245301397697</v>
       </c>
       <c r="O15">
@@ -2098,7 +2022,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1">
         <v>10</v>
@@ -2106,7 +2030,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -2114,7 +2038,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1">
         <v>10000</v>
@@ -2125,7 +2049,7 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2149,11 +2073,11 @@
     </row>
     <row r="8" spans="1:4">
       <c r="C8">
-        <f t="shared" ref="C8:C47" si="0">C7+0.00001</f>
+        <f t="shared" ref="C8:C46" si="0">C7+0.00001</f>
         <v>2.0000000000000002E-5</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" ref="D8:D47" si="1">$B$2+($B$1-$B$2)*EXP(-$B$3*C8)</f>
+        <f t="shared" ref="D8:D46" si="1">$B$2+($B$1-$B$2)*EXP(-$B$3*C8)</f>
         <v>8.5498460246238537</v>
       </c>
     </row>
@@ -2550,7 +2474,7 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="O5" sqref="O5:P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2558,14 +2482,16 @@
     <col min="3" max="3" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.21875" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.88671875" customWidth="1"/>
+    <col min="9" max="9" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1">
         <v>10</v>
@@ -2599,17 +2525,11 @@
       <c r="K4" t="s">
         <v>8</v>
       </c>
-      <c r="L4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>10</v>
       </c>
-      <c r="O4" t="s">
-        <v>12</v>
-      </c>
       <c r="P4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -2640,14 +2560,8 @@
       <c r="K5">
         <v>0</v>
       </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
       <c r="O5">
-        <f>(H5+K5+M5)/3</f>
+        <f>(F5+I5+K5)/3</f>
         <v>0</v>
       </c>
       <c r="P5">
@@ -2668,29 +2582,23 @@
       <c r="F6">
         <v>-4.7081055578697999</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
+        <v>7.1536650933786005E-17</v>
+      </c>
+      <c r="H6" s="1">
+        <v>-8.4884204693395003E-17</v>
+      </c>
+      <c r="I6" s="1">
         <v>-4.7081055578697999</v>
       </c>
-      <c r="H6">
-        <v>-4.7081055578697999</v>
-      </c>
-      <c r="I6" s="1">
-        <v>-4.6678096696557003E-18</v>
-      </c>
       <c r="J6" s="1">
-        <v>-2.7569977217991999E-17</v>
+        <v>6.0187153003885996E-16</v>
       </c>
       <c r="K6">
         <v>-4.7081055578697999</v>
       </c>
-      <c r="L6" s="1">
-        <v>5.9818910282569999E-16</v>
-      </c>
-      <c r="M6">
-        <v>-4.7081055578697999</v>
-      </c>
       <c r="O6">
-        <f t="shared" ref="O6:O15" si="0">(H6+K6+M6)/3</f>
+        <f t="shared" ref="O6:O15" si="0">(F6+I6+K6)/3</f>
         <v>-4.7081055578697999</v>
       </c>
       <c r="P6">
@@ -2703,7 +2611,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="1">
-        <v>1.1094692171643E-6</v>
+        <v>1.1094692173862999E-6</v>
       </c>
       <c r="E7" s="1">
         <v>7.5834437751850006E-5</v>
@@ -2711,25 +2619,19 @@
       <c r="F7">
         <v>-4.0627516583742</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
+        <v>5.0181934442420003E-17</v>
+      </c>
+      <c r="H7" s="1">
+        <v>6.3367366913978E-17</v>
+      </c>
+      <c r="I7" s="1">
         <v>-4.0627516583742</v>
       </c>
-      <c r="H7">
-        <v>-4.0627516583742</v>
-      </c>
-      <c r="I7" s="1">
-        <v>1.3288965271221001E-16</v>
-      </c>
       <c r="J7" s="1">
-        <v>7.6700568109365001E-17</v>
+        <v>2.2604952372787002E-16</v>
       </c>
       <c r="K7">
-        <v>-4.0627516583742</v>
-      </c>
-      <c r="L7" s="1">
-        <v>1.9859580961448001E-16</v>
-      </c>
-      <c r="M7">
         <v>-4.0627516583742</v>
       </c>
       <c r="O7">
@@ -2746,7 +2648,7 @@
         <v>3</v>
       </c>
       <c r="D8" s="1">
-        <v>1.2565080059757001E-6</v>
+        <v>1.2565080055316001E-6</v>
       </c>
       <c r="E8">
         <v>1.0934798898853E-4</v>
@@ -2754,25 +2656,19 @@
       <c r="F8">
         <v>-3.5354579930697998</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="1">
+        <v>-1.2068135908467E-16</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1.9095821864483E-16</v>
+      </c>
+      <c r="I8" s="1">
         <v>-3.5354579930697998</v>
       </c>
-      <c r="H8">
-        <v>-3.5354579930697998</v>
-      </c>
-      <c r="I8" s="1">
-        <v>2.0454708857051999E-16</v>
-      </c>
       <c r="J8" s="1">
-        <v>5.3736471353225001E-17</v>
+        <v>1.0620109900190001E-16</v>
       </c>
       <c r="K8">
-        <v>-3.5354579930697998</v>
-      </c>
-      <c r="L8" s="1">
-        <v>1.0329596950366E-16</v>
-      </c>
-      <c r="M8">
         <v>-3.5354579930697998</v>
       </c>
       <c r="O8">
@@ -2789,7 +2685,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="1">
-        <v>1.1911878592397E-6</v>
+        <v>1.1911878590176001E-6</v>
       </c>
       <c r="E9">
         <v>1.43021225539E-4</v>
@@ -2797,25 +2693,19 @@
       <c r="F9">
         <v>-3.1009676015438998</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1">
+        <v>-1.1112508559182E-18</v>
+      </c>
+      <c r="H9" s="1">
+        <v>4.0311900879634999E-17</v>
+      </c>
+      <c r="I9" s="1">
         <v>-3.1009676015438998</v>
       </c>
-      <c r="H9">
-        <v>-3.1009676015438998</v>
-      </c>
-      <c r="I9" s="1">
-        <v>-5.8774835269509998E-17</v>
-      </c>
       <c r="J9" s="1">
-        <v>-4.4449583286180998E-17</v>
+        <v>-1.6000687489357E-16</v>
       </c>
       <c r="K9">
-        <v>-3.1009676015438998</v>
-      </c>
-      <c r="L9" s="1">
-        <v>3.6581958629619998E-17</v>
-      </c>
-      <c r="M9">
         <v>-3.1009676015438998</v>
       </c>
       <c r="O9">
@@ -2840,25 +2730,19 @@
       <c r="F10">
         <v>-2.7407593266718999</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="1">
+        <v>5.9241688378645005E-16</v>
+      </c>
+      <c r="H10" s="1">
+        <v>-1.5717711066668E-17</v>
+      </c>
+      <c r="I10" s="1">
         <v>-2.7407593266718999</v>
       </c>
-      <c r="H10">
-        <v>-2.7407593266718999</v>
-      </c>
-      <c r="I10" s="1">
-        <v>5.3401310006858002E-16</v>
-      </c>
       <c r="J10" s="1">
-        <v>5.9714242902435999E-17</v>
+        <v>-4.2179990911369001E-16</v>
       </c>
       <c r="K10">
-        <v>-2.7407593266718999</v>
-      </c>
-      <c r="L10" s="1">
-        <v>3.7145939687263E-16</v>
-      </c>
-      <c r="M10">
         <v>-2.7407593266718999</v>
       </c>
       <c r="O10">
@@ -2883,25 +2767,19 @@
       <c r="F11">
         <v>-2.4408237756824001</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
+        <v>1.5796981589382E-16</v>
+      </c>
+      <c r="H11" s="1">
+        <v>-2.8643275626583998E-16</v>
+      </c>
+      <c r="I11" s="1">
         <v>-2.4408237756824001</v>
       </c>
-      <c r="H11">
-        <v>-2.4408237756824001</v>
-      </c>
-      <c r="I11" s="1">
-        <v>-1.4533833005442999E-16</v>
-      </c>
       <c r="J11" s="1">
-        <v>3.8069455489525002E-16</v>
+        <v>-5.1506963043695999E-16</v>
       </c>
       <c r="K11">
-        <v>-2.4408237756824001</v>
-      </c>
-      <c r="L11" s="1">
-        <v>-5.1816571164934997E-16</v>
-      </c>
-      <c r="M11">
         <v>-2.4408237756824001</v>
       </c>
       <c r="O11">
@@ -2918,7 +2796,7 @@
         <v>7</v>
       </c>
       <c r="D12" s="1">
-        <v>5.1287689051271001E-7</v>
+        <v>5.1287689029066996E-7</v>
       </c>
       <c r="E12">
         <v>2.4471674944074998E-4</v>
@@ -2926,25 +2804,19 @@
       <c r="F12">
         <v>-2.1902903907334998</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="1">
+        <v>1.7230468191087E-16</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1.2152549294017999E-16</v>
+      </c>
+      <c r="I12" s="1">
         <v>-2.1902903907334998</v>
       </c>
-      <c r="H12">
-        <v>-2.1902903907334998</v>
-      </c>
-      <c r="I12" s="1">
-        <v>5.3709742060880001E-16</v>
-      </c>
       <c r="J12" s="1">
-        <v>6.1729753795971002E-16</v>
+        <v>-5.8112996758932996E-16</v>
       </c>
       <c r="K12">
-        <v>-2.1902903907334998</v>
-      </c>
-      <c r="L12" s="1">
-        <v>-3.9057569362415999E-16</v>
-      </c>
-      <c r="M12">
         <v>-2.1902903907334998</v>
       </c>
       <c r="O12">
@@ -2961,7 +2833,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="1">
-        <v>3.2827704221638001E-7</v>
+        <v>3.2827704243843001E-7</v>
       </c>
       <c r="E13">
         <v>2.7877665760165998E-4</v>
@@ -2969,25 +2841,19 @@
       <c r="F13">
         <v>-1.9805510157838</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="1">
+        <v>2.2968188620986998E-16</v>
+      </c>
+      <c r="H13" s="1">
+        <v>2.3540560079365E-16</v>
+      </c>
+      <c r="I13" s="1">
         <v>-1.9805510157838</v>
       </c>
-      <c r="H13">
-        <v>-1.9805510157838</v>
-      </c>
-      <c r="I13" s="1">
-        <v>-1.3227396788635001E-16</v>
-      </c>
       <c r="J13" s="1">
-        <v>5.4599171349081999E-17</v>
+        <v>-2.5190413973461E-17</v>
       </c>
       <c r="K13">
-        <v>-1.9805510157838</v>
-      </c>
-      <c r="L13" s="1">
-        <v>1.3313853473926E-16</v>
-      </c>
-      <c r="M13">
         <v>-1.9805510157838</v>
       </c>
       <c r="O13">
@@ -3012,25 +2878,19 @@
       <c r="F14">
         <v>-1.8046804281233999</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="1">
+        <v>-3.2824213309943001E-16</v>
+      </c>
+      <c r="H14" s="1">
+        <v>9.6577095534788999E-17</v>
+      </c>
+      <c r="I14" s="1">
         <v>-1.8046804281233999</v>
       </c>
-      <c r="H14">
-        <v>-1.8046804281233999</v>
-      </c>
-      <c r="I14" s="1">
-        <v>5.8589039446427997E-17</v>
-      </c>
       <c r="J14" s="1">
-        <v>-1.1129317325552E-16</v>
+        <v>1.6063415630075999E-16</v>
       </c>
       <c r="K14">
-        <v>-1.8046804281233999</v>
-      </c>
-      <c r="L14" s="1">
-        <v>2.1575941704438001E-16</v>
-      </c>
-      <c r="M14">
         <v>-1.8046804281233999</v>
       </c>
       <c r="O14">
@@ -3047,7 +2907,7 @@
         <v>10</v>
       </c>
       <c r="D15" s="1">
-        <v>1.1059376503475E-7</v>
+        <v>1.1059376436862E-7</v>
       </c>
       <c r="E15">
         <v>3.4706153617313997E-4</v>
@@ -3055,25 +2915,19 @@
       <c r="F15">
         <v>-1.6570397488452999</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="1">
+        <v>4.7203319075413004E-16</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1.4008992482396E-17</v>
+      </c>
+      <c r="I15" s="1">
         <v>-1.6570397488452999</v>
       </c>
-      <c r="H15">
-        <v>-1.6570397488452999</v>
-      </c>
-      <c r="I15" s="1">
-        <v>3.5755043866335998E-16</v>
-      </c>
       <c r="J15" s="1">
-        <v>3.4890916717223001E-16</v>
+        <v>2.7632181497804998E-16</v>
       </c>
       <c r="K15">
-        <v>-1.6570397488452999</v>
-      </c>
-      <c r="L15" s="1">
-        <v>4.2578865146064998E-16</v>
-      </c>
-      <c r="M15">
         <v>-1.6570397488452999</v>
       </c>
       <c r="O15">
@@ -3102,7 +2956,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B1">
         <v>60</v>
@@ -3110,7 +2964,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -3118,7 +2972,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1">
         <v>5000</v>
@@ -3129,7 +2983,7 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -3153,7 +3007,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="C8">
-        <f t="shared" ref="C8:C47" si="0">C7+0.00001</f>
+        <f t="shared" ref="C8:C46" si="0">C7+0.00001</f>
         <v>2.0000000000000002E-5</v>
       </c>
       <c r="D8" s="1">

</xml_diff>

<commit_message>
Tests of the custom returnMap of Mohr-Coulomb.
Also a number of tests trivially re-golded so they can use the custom returnMap.

Also a number of tests modified because they had a much too large ep_plastic_tolerance.

Fixes #6242
</commit_message>
<xml_diff>
--- a/modules/tensor_mechanics/tests/mohr_coulomb/hard1_2.xlsx
+++ b/modules/tensor_mechanics/tests/mohr_coulomb/hard1_2.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\moose\projects_andy\moose\modules\tensor_mechanics\tests\mohr_coulomb\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="192" yWindow="24" windowWidth="22020" windowHeight="11904" activeTab="3"/>
+    <workbookView xWindow="192" yWindow="24" windowWidth="22020" windowHeight="11904" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="cohesion" sheetId="4" r:id="rId1"/>
     <sheet name="small_deform_hard1" sheetId="1" r:id="rId2"/>
-    <sheet name="expected1" sheetId="2" r:id="rId3"/>
-    <sheet name="friction" sheetId="7" r:id="rId4"/>
-    <sheet name="small_deform_hard2" sheetId="5" r:id="rId5"/>
-    <sheet name="expected2" sheetId="6" r:id="rId6"/>
+    <sheet name="planar_hard1" sheetId="8" r:id="rId3"/>
+    <sheet name="expected1" sheetId="2" r:id="rId4"/>
+    <sheet name="friction" sheetId="7" r:id="rId5"/>
+    <sheet name="small_deform_hard2" sheetId="5" r:id="rId6"/>
+    <sheet name="planar_hard2" sheetId="11" r:id="rId7"/>
+    <sheet name="expected2" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames>
+    <definedName name="small_deform_hard1" localSheetId="2">planar_hard1!$C$4:$K$14</definedName>
+    <definedName name="small_deform_hard1" localSheetId="6">planar_hard2!$C$4:$K$14</definedName>
     <definedName name="small_deform_hard1" localSheetId="1">small_deform_hard1!$C$4:$K$15</definedName>
-    <definedName name="small_deform_hard1" localSheetId="4">small_deform_hard2!$C$4:$K$15</definedName>
+    <definedName name="small_deform_hard1" localSheetId="5">small_deform_hard2!$C$4:$K$15</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -58,11 +67,45 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="3" name="small_deform_hard111" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="L:\moose\projects_andy\moose\modules\tensor_mechanics\tests\mohr_coulomb\planar_hard2.csv" comma="1">
+      <textFields count="11">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" name="small_deform_hard12" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="L:\moose\projects_andy\moose\modules\tensor_mechanics\tests\mohr_coulomb\gold\planar_hard1.csv" comma="1">
+      <textFields count="11">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="19">
   <si>
     <t>time</t>
   </si>
@@ -124,8 +167,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,12 +206,30 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-AU"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -201,11 +262,14 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -486,6 +550,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -585,16 +650,133 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="106490112"/>
-        <c:axId val="106496768"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>MOOSE (custom returnMap)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>planar_hard1!$E$5:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3.0596148821033001E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.5865996252190994E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0087998522363E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3571707632128999E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.7043094130129999E-4</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>2.0505852182828001E-4</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>2.3962546668750999E-4</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>2.7414969269645001E-4</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>3.0864376916657E-4</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>3.4311654052018999E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>planar_hard1!$P$5:$P$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>7.891319836551772</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.1403551913040317</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.9172508685762155</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0591036741269599</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.4551836733951662</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.0292767008745787</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.7284668745122072</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.5157900968643028</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.3653146835999399</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.2587937507886986</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="221134984"/>
+        <c:axId val="221135376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="106490112"/>
+        <c:axId val="221134984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4.0000000000000018E-4"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -613,20 +795,24 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106496768"/>
+        <c:crossAx val="221135376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106496768"/>
+        <c:axId val="221135376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
           <c:min val="2"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -646,10 +832,13 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106490112"/>
+        <c:crossAx val="221134984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -657,15 +846,28 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-AU"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -698,11 +900,14 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -983,6 +1188,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1082,16 +1288,133 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="107203200"/>
-        <c:axId val="107213952"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>MOOSE (custom returnMap)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>planar_hard2!$E$5:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.2251340619915998E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.3490049061532998E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.4642952469833995E-5</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>1.156865071056E-4</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>1.4661066210054001E-4</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>1.7741637738101E-4</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>2.081138773632E-4</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>2.3872118829736E-4</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>2.6926273943572E-4</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>2.9976793417489E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>planar_hard2!$P$5:$P$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>54.735452210722997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>48.266420429822077</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42.746898149579863</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38.03883385945916</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34.021990928584025</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30.592792275005383</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27.662674494019864</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25.156311944911049</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.009883300749653</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21.169460940065239</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="221136552"/>
+        <c:axId val="221136944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="107203200"/>
+        <c:axId val="221136552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4.0000000000000029E-4"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1110,20 +1433,24 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107213952"/>
+        <c:crossAx val="221136944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="107213952"/>
+        <c:axId val="221136944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
           <c:min val="15"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -1143,10 +1470,13 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107203200"/>
+        <c:crossAx val="221136552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1154,8 +1484,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
 </c:chartSpace>
 </file>
@@ -1164,7 +1497,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1175,7 +1508,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="121" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1186,7 +1519,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9282545" cy="6051917"/>
+    <xdr:ext cx="9276522" cy="6042991"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -1213,7 +1546,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9282545" cy="6051917"/>
+    <xdr:ext cx="9274432" cy="6034216"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -1241,7 +1574,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="small_deform_hard1" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="small_deform_hard1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="small_deform_hard1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1287,7 +1628,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1319,9 +1660,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1353,6 +1695,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1528,14 +1871,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
@@ -1546,7 +1889,7 @@
     <col min="13" max="13" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -1555,7 +1898,7 @@
         <v>1.0471975511965976</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1563,7 +1906,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>0</v>
       </c>
@@ -1598,7 +1941,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C5">
         <v>0</v>
       </c>
@@ -1635,7 +1978,7 @@
         <v>7.9999999999999982</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C6">
         <v>1</v>
       </c>
@@ -1672,7 +2015,7 @@
         <v>7.6505157131537773</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>2</v>
       </c>
@@ -1709,7 +2052,7 @@
         <v>5.9373909839564361</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>3</v>
       </c>
@@ -1746,7 +2089,7 @@
         <v>4.7582446220803964</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>4</v>
       </c>
@@ -1783,7 +2126,7 @@
         <v>3.939144088566005</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C10">
         <v>5</v>
       </c>
@@ -1820,7 +2163,7 @@
         <v>3.3666311346533835</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C11">
         <v>6</v>
       </c>
@@ -1857,7 +2200,7 @@
         <v>2.9647816150739632</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C12">
         <v>7</v>
       </c>
@@ -1894,7 +2237,7 @@
         <v>2.6818992255101013</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C13">
         <v>8</v>
       </c>
@@ -1931,7 +2274,7 @@
         <v>2.4823598481213955</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C14">
         <v>9</v>
       </c>
@@ -1968,7 +2311,7 @@
         <v>2.3414090810093913</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C15">
         <v>10</v>
       </c>
@@ -2011,16 +2354,455 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="8" width="8.88671875" customWidth="1"/>
+    <col min="9" max="9" width="12" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1">
+        <f>60*PI()/180</f>
+        <v>1.0471975511965976</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" t="s">
+        <v>8</v>
+      </c>
+      <c r="O4" t="s">
+        <v>10</v>
+      </c>
+      <c r="P4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>-4.4408920985006E-16</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3.0596148821033001E-5</v>
+      </c>
+      <c r="F5">
+        <v>4.5560556318946004</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>4.5560556318946004</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>4.5560556318946004</v>
+      </c>
+      <c r="O5">
+        <f>(F5+I5+K5)/3</f>
+        <v>4.5560556318946004</v>
+      </c>
+      <c r="P5">
+        <f>O5*SIN($B$1)/COS($B$1)</f>
+        <v>7.891319836551772</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>6.5865996252190994E-5</v>
+      </c>
+      <c r="F6">
+        <v>3.5451357226193001</v>
+      </c>
+      <c r="G6" s="1">
+        <v>-1.3877787807814001E-17</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>3.5451357226193001</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>3.5451357226193001</v>
+      </c>
+      <c r="O6">
+        <f t="shared" ref="O6:O14" si="0">(F6+I6+K6)/3</f>
+        <v>3.5451357226193001</v>
+      </c>
+      <c r="P6">
+        <f t="shared" ref="P6:P14" si="1">O6*SIN($B$1)/COS($B$1)</f>
+        <v>6.1403551913040317</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1.0087998522363E-4</v>
+      </c>
+      <c r="F7">
+        <v>2.8389761126453998</v>
+      </c>
+      <c r="G7" s="1">
+        <v>2.0816681711721999E-17</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>2.8389761126453998</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>2.8389761126453998</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>2.8389761126453998</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="1"/>
+        <v>4.9172508685762155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1.3571707632128999E-4</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2.3435245989258</v>
+      </c>
+      <c r="G8" s="1">
+        <v>2.7755575615629E-17</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>2.3435245989258</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>2.3435245989258</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>2.3435245989258</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="1"/>
+        <v>4.0591036741269599</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1.7043094130129999E-4</v>
+      </c>
+      <c r="F9">
+        <v>1.9948512239342999</v>
+      </c>
+      <c r="G9" s="1">
+        <v>-1.0364972768961E-16</v>
+      </c>
+      <c r="H9" s="1">
+        <v>-1.3403449357351999E-17</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1.9948512239342999</v>
+      </c>
+      <c r="J9" s="1">
+        <v>-2.0816681711721999E-17</v>
+      </c>
+      <c r="K9">
+        <v>1.9948512239342999</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>1.9948512239342999</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="1"/>
+        <v>3.4551836733951662</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>2.0505852182828001E-4</v>
+      </c>
+      <c r="F10">
+        <v>1.7489537186998001</v>
+      </c>
+      <c r="G10" s="1">
+        <v>-3.1210502497710998E-17</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1.1275702593849E-17</v>
+      </c>
+      <c r="I10" s="1">
+        <v>1.7489537186998001</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1.4745149545802999E-17</v>
+      </c>
+      <c r="K10">
+        <v>1.7489537186998001</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>1.7489537186998001</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="1"/>
+        <v>3.0292767008745787</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>2.3962546668750999E-4</v>
+      </c>
+      <c r="F11">
+        <v>1.5752810844745999</v>
+      </c>
+      <c r="G11" s="1">
+        <v>-1.2359904766335E-17</v>
+      </c>
+      <c r="H11" s="1">
+        <v>2.168404344971E-19</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1.5752810844745999</v>
+      </c>
+      <c r="J11" s="1">
+        <v>-1.3877787807814001E-17</v>
+      </c>
+      <c r="K11">
+        <v>1.5752810844745999</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="0"/>
+        <v>1.5752810844745999</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="1"/>
+        <v>2.7284668745122072</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>2.7414969269645001E-4</v>
+      </c>
+      <c r="F12">
+        <v>1.4524920896492</v>
+      </c>
+      <c r="G12" s="1">
+        <v>4.8572257327350999E-17</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1.4524920896492</v>
+      </c>
+      <c r="J12" s="1">
+        <v>6.9388939039071999E-18</v>
+      </c>
+      <c r="K12">
+        <v>1.4524920896492</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>1.4524920896492002</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="1"/>
+        <v>2.5157900968643028</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>9</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>3.0864376916657E-4</v>
+      </c>
+      <c r="F13">
+        <v>1.3656150692946001</v>
+      </c>
+      <c r="G13" s="1">
+        <v>4.3368086899419999E-17</v>
+      </c>
+      <c r="H13" s="1">
+        <v>3.3610267347051E-18</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1.3656150692946001</v>
+      </c>
+      <c r="J13" s="1">
+        <v>6.9388939039071999E-18</v>
+      </c>
+      <c r="K13">
+        <v>1.3656150692946001</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="0"/>
+        <v>1.3656150692946001</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="1"/>
+        <v>2.3653146835999399</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>3.4311654052018999E-4</v>
+      </c>
+      <c r="F14">
+        <v>1.3041151800616999</v>
+      </c>
+      <c r="G14" s="1">
+        <v>-6.4618449480136003E-17</v>
+      </c>
+      <c r="H14" s="1">
+        <v>-1.3877787807814001E-17</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1.3041151800616999</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1.1275702593849E-17</v>
+      </c>
+      <c r="K14">
+        <v>1.3041151800616999</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="0"/>
+        <v>1.3041151800616999</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="1"/>
+        <v>2.2587937507886986</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="C6" sqref="C6:D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -2028,7 +2810,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -2036,7 +2818,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2044,7 +2826,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>2</v>
       </c>
@@ -2052,7 +2834,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C6">
         <v>0</v>
       </c>
@@ -2061,7 +2843,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C7">
         <f>C6+0.00001</f>
         <v>1.0000000000000001E-5</v>
@@ -2071,7 +2853,7 @@
         <v>9.2386993442876761</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C8">
         <f t="shared" ref="C8:C46" si="0">C7+0.00001</f>
         <v>2.0000000000000002E-5</v>
@@ -2081,7 +2863,7 @@
         <v>8.5498460246238537</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C9">
         <f t="shared" si="0"/>
         <v>3.0000000000000004E-5</v>
@@ -2091,7 +2873,7 @@
         <v>7.926545765453743</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C10">
         <f t="shared" si="0"/>
         <v>4.0000000000000003E-5</v>
@@ -2101,7 +2883,7 @@
         <v>7.3625603682851146</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C11">
         <f t="shared" si="0"/>
         <v>5.0000000000000002E-5</v>
@@ -2111,7 +2893,7 @@
         <v>6.8522452777010674</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C12">
         <f t="shared" si="0"/>
         <v>6.0000000000000002E-5</v>
@@ -2121,7 +2903,7 @@
         <v>6.3904930887522111</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C13">
         <f t="shared" si="0"/>
         <v>7.0000000000000007E-5</v>
@@ -2131,7 +2913,7 @@
         <v>5.9726824303312753</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C14">
         <f t="shared" si="0"/>
         <v>8.0000000000000007E-5</v>
@@ -2141,7 +2923,7 @@
         <v>5.5946317129377725</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C15">
         <f t="shared" si="0"/>
         <v>9.0000000000000006E-5</v>
@@ -2151,7 +2933,7 @@
         <v>5.2525572779247929</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C16">
         <f t="shared" si="0"/>
         <v>1E-4</v>
@@ -2161,7 +2943,7 @@
         <v>4.9430355293715387</v>
       </c>
     </row>
-    <row r="17" spans="3:4">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C17">
         <f t="shared" si="0"/>
         <v>1.1E-4</v>
@@ -2171,7 +2953,7 @@
         <v>4.662968669584636</v>
       </c>
     </row>
-    <row r="18" spans="3:4">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C18">
         <f t="shared" si="0"/>
         <v>1.2E-4</v>
@@ -2181,7 +2963,7 @@
         <v>4.4095536952976175</v>
       </c>
     </row>
-    <row r="19" spans="3:4">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C19">
         <f t="shared" si="0"/>
         <v>1.3000000000000002E-4</v>
@@ -2191,7 +2973,7 @@
         <v>4.1802543442721003</v>
       </c>
     </row>
-    <row r="20" spans="3:4">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C20">
         <f t="shared" si="0"/>
         <v>1.4000000000000001E-4</v>
@@ -2201,7 +2983,7 @@
         <v>3.9727757115328517</v>
       </c>
     </row>
-    <row r="21" spans="3:4">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C21">
         <f t="shared" si="0"/>
         <v>1.5000000000000001E-4</v>
@@ -2211,7 +2993,7 @@
         <v>3.7850412811874383</v>
       </c>
     </row>
-    <row r="22" spans="3:4">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C22">
         <f t="shared" si="0"/>
         <v>1.6000000000000001E-4</v>
@@ -2221,7 +3003,7 @@
         <v>3.6151721439572428</v>
       </c>
     </row>
-    <row r="23" spans="3:4">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C23">
         <f t="shared" si="0"/>
         <v>1.7000000000000001E-4</v>
@@ -2231,7 +3013,7 @@
         <v>3.4614681924218766</v>
       </c>
     </row>
-    <row r="24" spans="3:4">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C24">
         <f t="shared" si="0"/>
         <v>1.8000000000000001E-4</v>
@@ -2241,7 +3023,7 @@
         <v>3.3223911057726925</v>
       </c>
     </row>
-    <row r="25" spans="3:4">
+    <row r="25" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C25">
         <f t="shared" si="0"/>
         <v>1.9000000000000001E-4</v>
@@ -2251,7 +3033,7 @@
         <v>3.1965489537810803</v>
       </c>
     </row>
-    <row r="26" spans="3:4">
+    <row r="26" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C26">
         <f t="shared" si="0"/>
         <v>2.0000000000000001E-4</v>
@@ -2261,7 +3043,7 @@
         <v>3.0826822658929016</v>
       </c>
     </row>
-    <row r="27" spans="3:4">
+    <row r="27" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C27">
         <f t="shared" si="0"/>
         <v>2.1000000000000001E-4</v>
@@ -2271,7 +3053,7 @@
         <v>2.9796514260238554</v>
       </c>
     </row>
-    <row r="28" spans="3:4">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C28">
         <f t="shared" si="0"/>
         <v>2.2000000000000001E-4</v>
@@ -2281,7 +3063,7 @@
         <v>2.8864252668986712</v>
       </c>
     </row>
-    <row r="29" spans="3:4">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C29">
         <f t="shared" si="0"/>
         <v>2.3000000000000001E-4</v>
@@ -2291,7 +3073,7 @@
         <v>2.8020707497824295</v>
       </c>
     </row>
-    <row r="30" spans="3:4">
+    <row r="30" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C30">
         <f t="shared" si="0"/>
         <v>2.4000000000000001E-4</v>
@@ -2301,7 +3083,7 @@
         <v>2.7257436263153001</v>
       </c>
     </row>
-    <row r="31" spans="3:4">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C31">
         <f t="shared" si="0"/>
         <v>2.5000000000000001E-4</v>
@@ -2311,7 +3093,7 @@
         <v>2.6566799889911903</v>
       </c>
     </row>
-    <row r="32" spans="3:4">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C32">
         <f t="shared" si="0"/>
         <v>2.6000000000000003E-4</v>
@@ -2321,7 +3103,7 @@
         <v>2.5941886257146707</v>
       </c>
     </row>
-    <row r="33" spans="3:4">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C33">
         <f t="shared" si="0"/>
         <v>2.7000000000000006E-4</v>
@@ -2331,7 +3113,7 @@
         <v>2.5376441019179978</v>
       </c>
     </row>
-    <row r="34" spans="3:4">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C34">
         <f t="shared" si="0"/>
         <v>2.8000000000000008E-4</v>
@@ -2341,7 +3123,7 @@
         <v>2.4864805010017434</v>
       </c>
     </row>
-    <row r="35" spans="3:4">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C35">
         <f t="shared" si="0"/>
         <v>2.9000000000000011E-4</v>
@@ -2351,7 +3133,7 @@
         <v>2.4401857604512571</v>
       </c>
     </row>
-    <row r="36" spans="3:4">
+    <row r="36" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C36">
         <f t="shared" si="0"/>
         <v>3.0000000000000014E-4</v>
@@ -2361,7 +3143,7 @@
         <v>2.3982965469429112</v>
       </c>
     </row>
-    <row r="37" spans="3:4">
+    <row r="37" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C37">
         <f t="shared" si="0"/>
         <v>3.1000000000000016E-4</v>
@@ -2371,7 +3153,7 @@
         <v>2.360393619148462</v>
       </c>
     </row>
-    <row r="38" spans="3:4">
+    <row r="38" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C38">
         <f t="shared" si="0"/>
         <v>3.2000000000000019E-4</v>
@@ -2381,7 +3163,7 @@
         <v>2.3260976318269293</v>
       </c>
     </row>
-    <row r="39" spans="3:4">
+    <row r="39" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C39">
         <f t="shared" si="0"/>
         <v>3.3000000000000022E-4</v>
@@ -2391,7 +3173,7 @@
         <v>2.2950653392099194</v>
       </c>
     </row>
-    <row r="40" spans="3:4">
+    <row r="40" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C40">
         <f t="shared" si="0"/>
         <v>3.4000000000000024E-4</v>
@@ -2401,7 +3183,7 @@
         <v>2.2669861596826077</v>
       </c>
     </row>
-    <row r="41" spans="3:4">
+    <row r="41" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C41">
         <f t="shared" si="0"/>
         <v>3.5000000000000027E-4</v>
@@ -2411,7 +3193,7 @@
         <v>2.2415790673785474</v>
       </c>
     </row>
-    <row r="42" spans="3:4">
+    <row r="42" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C42">
         <f t="shared" si="0"/>
         <v>3.6000000000000029E-4</v>
@@ -2421,7 +3203,7 @@
         <v>2.2185897795783398</v>
       </c>
     </row>
-    <row r="43" spans="3:4">
+    <row r="43" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C43">
         <f t="shared" si="0"/>
         <v>3.7000000000000032E-4</v>
@@ -2431,7 +3213,7 @@
         <v>2.1977882117627145</v>
       </c>
     </row>
-    <row r="44" spans="3:4">
+    <row r="44" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C44">
         <f t="shared" si="0"/>
         <v>3.8000000000000035E-4</v>
@@ -2441,7 +3223,7 @@
         <v>2.1789661748493243</v>
       </c>
     </row>
-    <row r="45" spans="3:4">
+    <row r="45" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C45">
         <f t="shared" si="0"/>
         <v>3.9000000000000037E-4</v>
@@ -2451,7 +3233,7 @@
         <v>2.1619352915664343</v>
       </c>
     </row>
-    <row r="46" spans="3:4">
+    <row r="46" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C46">
         <f t="shared" si="0"/>
         <v>4.000000000000004E-4</v>
@@ -2461,7 +3243,7 @@
         <v>2.1465251111098729</v>
       </c>
     </row>
-    <row r="47" spans="3:4">
+    <row r="47" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D47" s="1"/>
     </row>
   </sheetData>
@@ -2469,15 +3251,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O5" sqref="O5:P15"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.21875" customWidth="1"/>
@@ -2489,7 +3271,7 @@
     <col min="13" max="13" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -2497,7 +3279,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>0</v>
       </c>
@@ -2532,7 +3314,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C5">
         <v>0</v>
       </c>
@@ -2569,7 +3351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C6">
         <v>1</v>
       </c>
@@ -2606,7 +3388,7 @@
         <v>50.423102668677068</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>2</v>
       </c>
@@ -2643,7 +3425,7 @@
         <v>44.221371941192665</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>3</v>
       </c>
@@ -2680,7 +3462,7 @@
         <v>38.941668025064295</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>4</v>
       </c>
@@ -2717,7 +3499,7 @@
         <v>34.456987876737472</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C10">
         <v>5</v>
       </c>
@@ -2754,7 +3536,7 @@
         <v>30.654033874341042</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C11">
         <v>6</v>
       </c>
@@ -2791,7 +3573,7 @@
         <v>27.433382895118211</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C12">
         <v>7</v>
       </c>
@@ -2828,7 +3610,7 @@
         <v>24.708688095299166</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C13">
         <v>8</v>
       </c>
@@ -2865,7 +3647,7 @@
         <v>22.405487957106242</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C14">
         <v>9</v>
       </c>
@@ -2902,7 +3684,7 @@
         <v>20.459893758385203</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C15">
         <v>10</v>
       </c>
@@ -2944,17 +3726,455 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O5" sqref="O5:P14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="8" width="8.88671875" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" t="s">
+        <v>8</v>
+      </c>
+      <c r="O4" t="s">
+        <v>10</v>
+      </c>
+      <c r="P4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2.2251340619915998E-5</v>
+      </c>
+      <c r="F5">
+        <v>7.0711092041369996</v>
+      </c>
+      <c r="G5" s="1">
+        <v>4.1633363423443E-17</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>7.0711092041369996</v>
+      </c>
+      <c r="J5" s="1">
+        <v>-6.2907306603042006E-39</v>
+      </c>
+      <c r="K5">
+        <v>7.0711092041369996</v>
+      </c>
+      <c r="O5">
+        <f>(F5+I5+K5)/3</f>
+        <v>7.0711092041369996</v>
+      </c>
+      <c r="P5">
+        <f>ATAN($B$1/O5)*180/PI()</f>
+        <v>54.735452210722997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>8.8817841970012997E-16</v>
+      </c>
+      <c r="E6" s="1">
+        <v>5.3490049061532998E-5</v>
+      </c>
+      <c r="F6">
+        <v>8.9201936252721996</v>
+      </c>
+      <c r="G6" s="1">
+        <v>-3.1115076389305999E-61</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>8.9201936252721996</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1.0928427348869E-38</v>
+      </c>
+      <c r="K6">
+        <v>8.9201936252721996</v>
+      </c>
+      <c r="O6">
+        <f t="shared" ref="O6:O14" si="0">(F6+I6+K6)/3</f>
+        <v>8.9201936252721996</v>
+      </c>
+      <c r="P6">
+        <f t="shared" ref="P6:P14" si="1">ATAN($B$1/O6)*180/PI()</f>
+        <v>48.266420429822077</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>8.4642952469833995E-5</v>
+      </c>
+      <c r="F7">
+        <v>10.819114056230999</v>
+      </c>
+      <c r="G7" s="1">
+        <v>-3.3306690738755002E-16</v>
+      </c>
+      <c r="H7" s="1">
+        <v>5.8774717541113997E-39</v>
+      </c>
+      <c r="I7" s="1">
+        <v>10.819114056230999</v>
+      </c>
+      <c r="J7" s="1">
+        <v>-1.0873322745106001E-37</v>
+      </c>
+      <c r="K7">
+        <v>10.819114056230999</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>10.819114056230999</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="1"/>
+        <v>42.746898149579863</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1">
+        <v>-7.7715611723760997E-16</v>
+      </c>
+      <c r="E8">
+        <v>1.156865071056E-4</v>
+      </c>
+      <c r="F8">
+        <v>12.781550317532</v>
+      </c>
+      <c r="G8" s="1">
+        <v>6.9388939039072E-17</v>
+      </c>
+      <c r="H8" s="1">
+        <v>-1.3877787807814001E-17</v>
+      </c>
+      <c r="I8" s="1">
+        <v>12.781550317532</v>
+      </c>
+      <c r="J8" s="1">
+        <v>-1.1102230246251999E-16</v>
+      </c>
+      <c r="K8">
+        <v>12.781550317532</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>12.781550317532</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="1"/>
+        <v>38.03883385945916</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1.4661066210054001E-4</v>
+      </c>
+      <c r="F9">
+        <v>14.813342339567001</v>
+      </c>
+      <c r="G9" s="1">
+        <v>-5.6639890471619999E-16</v>
+      </c>
+      <c r="H9" s="1">
+        <v>-2.2204460492503E-16</v>
+      </c>
+      <c r="I9" s="1">
+        <v>14.813342339567001</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1.6653345369377001E-16</v>
+      </c>
+      <c r="K9">
+        <v>14.813342339567001</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>14.813342339567001</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="1"/>
+        <v>34.021990928584025</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1.7741637738101E-4</v>
+      </c>
+      <c r="F10">
+        <v>16.913932368373999</v>
+      </c>
+      <c r="G10" s="1">
+        <v>6.6613381477508998E-16</v>
+      </c>
+      <c r="H10" s="1">
+        <v>3.1918911957972999E-16</v>
+      </c>
+      <c r="I10" s="1">
+        <v>16.913932368373999</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1.1102230246251999E-16</v>
+      </c>
+      <c r="K10">
+        <v>16.913932368373999</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>16.913932368373999</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="1"/>
+        <v>30.592792275005383</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>2.081138773632E-4</v>
+      </c>
+      <c r="F11">
+        <v>19.077379626707</v>
+      </c>
+      <c r="G11" s="1">
+        <v>-7.3552275381416996E-16</v>
+      </c>
+      <c r="H11" s="1">
+        <v>-2.4980018054066002E-16</v>
+      </c>
+      <c r="I11" s="1">
+        <v>19.077379626707</v>
+      </c>
+      <c r="J11" s="1">
+        <v>-2.2204460492503E-16</v>
+      </c>
+      <c r="K11">
+        <v>19.077379626707</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="0"/>
+        <v>19.077379626707</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="1"/>
+        <v>27.662674494019864</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>2.3872118829736E-4</v>
+      </c>
+      <c r="F12">
+        <v>21.293210173034002</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1.6653345369377001E-16</v>
+      </c>
+      <c r="H12" s="1">
+        <v>-1.3877787807814001E-16</v>
+      </c>
+      <c r="I12" s="1">
+        <v>21.293210173034002</v>
+      </c>
+      <c r="J12" s="1">
+        <v>-4.7184478546568995E-16</v>
+      </c>
+      <c r="K12">
+        <v>21.293210173034002</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>21.293210173034002</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="1"/>
+        <v>25.156311944911049</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>9</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>2.6926273943572E-4</v>
+      </c>
+      <c r="F13">
+        <v>23.547229680977001</v>
+      </c>
+      <c r="G13" s="1">
+        <v>-8.3266726846886999E-17</v>
+      </c>
+      <c r="H13" s="1">
+        <v>6.9388939039072E-17</v>
+      </c>
+      <c r="I13" s="1">
+        <v>23.547229680977001</v>
+      </c>
+      <c r="J13" s="1">
+        <v>-5.5511151231258005E-16</v>
+      </c>
+      <c r="K13">
+        <v>23.547229680977001</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="0"/>
+        <v>23.547229680977001</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="1"/>
+        <v>23.009883300749653</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>2.9976793417489E-4</v>
+      </c>
+      <c r="F14">
+        <v>25.822353646951999</v>
+      </c>
+      <c r="G14" s="1">
+        <v>5.7592692347487996E-16</v>
+      </c>
+      <c r="H14" s="1">
+        <v>-1.1102230246251999E-16</v>
+      </c>
+      <c r="I14" s="1">
+        <v>25.822353646951999</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1.1102230246251999E-16</v>
+      </c>
+      <c r="K14">
+        <v>25.822353646951999</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="0"/>
+        <v>25.822353646951999</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="1"/>
+        <v>21.169460940065239</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:D46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -2962,7 +4182,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -2970,7 +4190,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -2978,7 +4198,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>2</v>
       </c>
@@ -2986,7 +4206,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C6">
         <v>0</v>
       </c>
@@ -2995,7 +4215,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C7">
         <f>C6+0.00001</f>
         <v>1.0000000000000001E-5</v>
@@ -3005,7 +4225,7 @@
         <v>57.561471225035703</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C8">
         <f t="shared" ref="C8:C46" si="0">C7+0.00001</f>
         <v>2.0000000000000002E-5</v>
@@ -3015,7 +4235,7 @@
         <v>55.241870901797974</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C9">
         <f t="shared" si="0"/>
         <v>3.0000000000000004E-5</v>
@@ -3025,7 +4245,7 @@
         <v>53.03539882125289</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C10">
         <f t="shared" si="0"/>
         <v>4.0000000000000003E-5</v>
@@ -3035,7 +4255,7 @@
         <v>50.936537653899094</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C11">
         <f t="shared" si="0"/>
         <v>5.0000000000000002E-5</v>
@@ -3045,7 +4265,7 @@
         <v>48.940039153570247</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C12">
         <f t="shared" si="0"/>
         <v>6.0000000000000002E-5</v>
@@ -3055,7 +4275,7 @@
         <v>47.040911034085894</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C13">
         <f t="shared" si="0"/>
         <v>7.0000000000000007E-5</v>
@@ -3065,7 +4285,7 @@
         <v>45.23440448593567</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C14">
         <f t="shared" si="0"/>
         <v>8.0000000000000007E-5</v>
@@ -3075,7 +4295,7 @@
         <v>43.516002301781967</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C15">
         <f t="shared" si="0"/>
         <v>9.0000000000000006E-5</v>
@@ -3085,7 +4305,7 @@
         <v>41.881407581088666</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C16">
         <f t="shared" si="0"/>
         <v>1E-4</v>
@@ -3095,7 +4315,7 @@
         <v>40.326532985631673</v>
       </c>
     </row>
-    <row r="17" spans="3:4">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C17">
         <f t="shared" si="0"/>
         <v>1.1E-4</v>
@@ -3105,7 +4325,7 @@
         <v>38.847490519024333</v>
       </c>
     </row>
-    <row r="18" spans="3:4">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C18">
         <f t="shared" si="0"/>
         <v>1.2E-4</v>
@@ -3115,7 +4335,7 @@
         <v>37.440581804701324</v>
       </c>
     </row>
-    <row r="19" spans="3:4">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C19">
         <f t="shared" si="0"/>
         <v>1.3000000000000002E-4</v>
@@ -3125,7 +4345,7 @@
         <v>36.102288838050796</v>
       </c>
     </row>
-    <row r="20" spans="3:4">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C20">
         <f t="shared" si="0"/>
         <v>1.4000000000000001E-4</v>
@@ -3135,7 +4355,7 @@
         <v>34.829265189570478</v>
       </c>
     </row>
-    <row r="21" spans="3:4">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C21">
         <f t="shared" si="0"/>
         <v>1.5000000000000001E-4</v>
@@ -3145,7 +4365,7 @@
         <v>33.618327637050733</v>
       </c>
     </row>
-    <row r="22" spans="3:4">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C22">
         <f t="shared" si="0"/>
         <v>1.6000000000000001E-4</v>
@@ -3155,7 +4375,7 @@
         <v>32.466448205861077</v>
       </c>
     </row>
-    <row r="23" spans="3:4">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C23">
         <f t="shared" si="0"/>
         <v>1.7000000000000001E-4</v>
@@ -3165,7 +4385,7 @@
         <v>31.370746597436334</v>
       </c>
     </row>
-    <row r="24" spans="3:4">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C24">
         <f t="shared" si="0"/>
         <v>1.8000000000000001E-4</v>
@@ -3175,7 +4395,7 @@
         <v>30.328482987029954</v>
       </c>
     </row>
-    <row r="25" spans="3:4">
+    <row r="25" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C25">
         <f t="shared" si="0"/>
         <v>1.9000000000000001E-4</v>
@@ -3185,7 +4405,7 @@
         <v>29.337051172725058</v>
       </c>
     </row>
-    <row r="26" spans="3:4">
+    <row r="26" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C26">
         <f t="shared" si="0"/>
         <v>2.0000000000000001E-4</v>
@@ -3195,7 +4415,7 @@
         <v>28.393972058572118</v>
       </c>
     </row>
-    <row r="27" spans="3:4">
+    <row r="27" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C27">
         <f t="shared" si="0"/>
         <v>2.1000000000000001E-4</v>
@@ -3205,7 +4425,7 @@
         <v>27.496887455557765</v>
       </c>
     </row>
-    <row r="28" spans="3:4">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C28">
         <f t="shared" si="0"/>
         <v>2.2000000000000001E-4</v>
@@ -3215,7 +4435,7 @@
         <v>26.643554184903977</v>
       </c>
     </row>
-    <row r="29" spans="3:4">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C29">
         <f t="shared" si="0"/>
         <v>2.3000000000000001E-4</v>
@@ -3225,7 +4445,7 @@
         <v>25.831838468952657</v>
       </c>
     </row>
-    <row r="30" spans="3:4">
+    <row r="30" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C30">
         <f t="shared" si="0"/>
         <v>2.4000000000000001E-4</v>
@@ -3235,7 +4455,7 @@
         <v>25.059710595610106</v>
       </c>
     </row>
-    <row r="31" spans="3:4">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C31">
         <f t="shared" si="0"/>
         <v>2.5000000000000001E-4</v>
@@ -3245,7 +4465,7 @@
         <v>24.325239843009506</v>
       </c>
     </row>
-    <row r="32" spans="3:4">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C32">
         <f t="shared" si="0"/>
         <v>2.6000000000000003E-4</v>
@@ -3255,7 +4475,7 @@
         <v>23.626589651700627</v>
       </c>
     </row>
-    <row r="33" spans="3:4">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C33">
         <f t="shared" si="0"/>
         <v>2.7000000000000006E-4</v>
@@ -3265,7 +4485,7 @@
         <v>22.962013032294571</v>
       </c>
     </row>
-    <row r="34" spans="3:4">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C34">
         <f t="shared" si="0"/>
         <v>2.8000000000000008E-4</v>
@@ -3275,7 +4495,7 @@
         <v>22.329848197080317</v>
       </c>
     </row>
-    <row r="35" spans="3:4">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C35">
         <f t="shared" si="0"/>
         <v>2.9000000000000011E-4</v>
@@ -3285,7 +4505,7 @@
         <v>21.728514404689875</v>
       </c>
     </row>
-    <row r="36" spans="3:4">
+    <row r="36" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C36">
         <f t="shared" si="0"/>
         <v>3.0000000000000014E-4</v>
@@ -3295,7 +4515,7 @@
         <v>21.156508007421486</v>
       </c>
     </row>
-    <row r="37" spans="3:4">
+    <row r="37" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C37">
         <f t="shared" si="0"/>
         <v>3.1000000000000016E-4</v>
@@ -3305,7 +4525,7 @@
         <v>20.612398691337145</v>
       </c>
     </row>
-    <row r="38" spans="3:4">
+    <row r="38" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C38">
         <f t="shared" si="0"/>
         <v>3.2000000000000019E-4</v>
@@ -3315,7 +4535,7 @@
         <v>20.094825899732761</v>
       </c>
     </row>
-    <row r="39" spans="3:4">
+    <row r="39" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C39">
         <f t="shared" si="0"/>
         <v>3.3000000000000022E-4</v>
@@ -3325,7 +4545,7 @@
         <v>19.602495431037696</v>
       </c>
     </row>
-    <row r="40" spans="3:4">
+    <row r="40" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C40">
         <f t="shared" si="0"/>
         <v>3.4000000000000024E-4</v>
@@ -3335,7 +4555,7 @@
         <v>19.13417620263672</v>
       </c>
     </row>
-    <row r="41" spans="3:4">
+    <row r="41" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C41">
         <f t="shared" si="0"/>
         <v>3.5000000000000027E-4</v>
@@ -3345,7 +4565,7 @@
         <v>18.688697172522247</v>
       </c>
     </row>
-    <row r="42" spans="3:4">
+    <row r="42" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C42">
         <f t="shared" si="0"/>
         <v>3.6000000000000029E-4</v>
@@ -3355,7 +4575,7 @@
         <v>18.264944411079316</v>
       </c>
     </row>
-    <row r="43" spans="3:4">
+    <row r="43" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C43">
         <f t="shared" si="0"/>
         <v>3.7000000000000032E-4</v>
@@ -3365,7 +4585,7 @@
         <v>17.861858315681367</v>
       </c>
     </row>
-    <row r="44" spans="3:4">
+    <row r="44" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C44">
         <f t="shared" si="0"/>
         <v>3.8000000000000035E-4</v>
@@ -3375,7 +4595,7 @@
         <v>17.478430961131743</v>
       </c>
     </row>
-    <row r="45" spans="3:4">
+    <row r="45" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C45">
         <f t="shared" si="0"/>
         <v>3.9000000000000037E-4</v>
@@ -3385,7 +4605,7 @@
         <v>17.113703579325666</v>
       </c>
     </row>
-    <row r="46" spans="3:4">
+    <row r="46" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C46">
         <f t="shared" si="0"/>
         <v>4.000000000000004E-4</v>
@@ -3395,7 +4615,7 @@
         <v>16.766764161830622</v>
       </c>
     </row>
-    <row r="47" spans="3:4">
+    <row r="47" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D47" s="1"/>
     </row>
   </sheetData>

</xml_diff>